<commit_message>
Final Project - Add Category
</commit_message>
<xml_diff>
--- a/src/test/java/haimai/datatest/dataTestProject.xlsx
+++ b/src/test/java/haimai/datatest/dataTestProject.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="addBrand" sheetId="1" r:id="rId1"/>
     <sheet name="editBrand" sheetId="3" r:id="rId2"/>
     <sheet name="delBrand" sheetId="4" r:id="rId3"/>
     <sheet name="addCategory" sheetId="2" r:id="rId4"/>
+    <sheet name="addProduct" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="80">
   <si>
     <t>name</t>
   </si>
@@ -159,6 +160,114 @@
   </si>
   <si>
     <t>Edit Brand 3 Hai</t>
+  </si>
+  <si>
+    <t>parentCat</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>filterAtt</t>
+  </si>
+  <si>
+    <t>Size</t>
+  </si>
+  <si>
+    <t>Digital</t>
+  </si>
+  <si>
+    <t>Physical</t>
+  </si>
+  <si>
+    <t>Wheel</t>
+  </si>
+  <si>
+    <t>Toy</t>
+  </si>
+  <si>
+    <t>Hot Categories</t>
+  </si>
+  <si>
+    <t>catName</t>
+  </si>
+  <si>
+    <t>productName</t>
+  </si>
+  <si>
+    <t>brandName</t>
+  </si>
+  <si>
+    <t>Hai product 1</t>
+  </si>
+  <si>
+    <t>Hai product 2</t>
+  </si>
+  <si>
+    <t>unit</t>
+  </si>
+  <si>
+    <t>kg</t>
+  </si>
+  <si>
+    <t>pc</t>
+  </si>
+  <si>
+    <t>minPurchaseQty</t>
+  </si>
+  <si>
+    <t>tag</t>
+  </si>
+  <si>
+    <t>hai</t>
+  </si>
+  <si>
+    <t>barcode</t>
+  </si>
+  <si>
+    <t>galleryFilePath</t>
+  </si>
+  <si>
+    <t>galleryFileName</t>
+  </si>
+  <si>
+    <t>videoProvider</t>
+  </si>
+  <si>
+    <t>videoLink</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=JZ9pHBEUWPo</t>
+  </si>
+  <si>
+    <t>Vimeo</t>
+  </si>
+  <si>
+    <t>Dailymotion</t>
+  </si>
+  <si>
+    <t>unitPrice</t>
+  </si>
+  <si>
+    <t>discount</t>
+  </si>
+  <si>
+    <t>percent</t>
+  </si>
+  <si>
+    <t>quantity</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>Description of Hai Product 1</t>
+  </si>
+  <si>
+    <t>Description of Hai Product 2</t>
+  </si>
+  <si>
+    <t>this is meta title</t>
   </si>
 </sst>
 </file>
@@ -501,8 +610,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -741,100 +850,315 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="A2" sqref="A2:A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" customWidth="1"/>
-    <col min="2" max="2" width="19.28515625" customWidth="1"/>
-    <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="14.85546875" customWidth="1"/>
-    <col min="5" max="5" width="15.85546875" customWidth="1"/>
-    <col min="6" max="6" width="14.28515625" customWidth="1"/>
-    <col min="7" max="7" width="34.42578125" customWidth="1"/>
-    <col min="8" max="8" width="13" customWidth="1"/>
+    <col min="1" max="2" width="13.5703125" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" customWidth="1"/>
+    <col min="5" max="5" width="18" customWidth="1"/>
+    <col min="6" max="6" width="14.85546875" customWidth="1"/>
+    <col min="7" max="7" width="15.85546875" customWidth="1"/>
+    <col min="8" max="8" width="14.28515625" customWidth="1"/>
+    <col min="9" max="9" width="34.42578125" customWidth="1"/>
+    <col min="10" max="10" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K1" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" s="4">
         <v>123</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="D2" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E2" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="F2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="G2" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="H2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="I2" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="J2" s="6" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K2" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" s="4">
         <v>456</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="D3" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E3" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="F3" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="G3" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="H3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="I3" s="7" t="s">
         <v>29</v>
       </c>
+      <c r="J3" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="P7" sqref="P7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="13.5703125" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" customWidth="1"/>
+    <col min="4" max="4" width="6.28515625" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" customWidth="1"/>
+    <col min="6" max="7" width="7.7109375" customWidth="1"/>
+    <col min="8" max="8" width="18" customWidth="1"/>
+    <col min="9" max="9" width="14.85546875" customWidth="1"/>
+    <col min="10" max="10" width="15.85546875" customWidth="1"/>
+    <col min="11" max="11" width="14.28515625" customWidth="1"/>
+    <col min="12" max="12" width="8.7109375" customWidth="1"/>
+    <col min="13" max="13" width="13" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E2" s="4">
+        <v>10</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="G2" s="4">
+        <v>98765</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="L2" s="7">
+        <v>200</v>
+      </c>
+      <c r="M2" s="6">
+        <v>30</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="O2">
+        <v>1000</v>
+      </c>
+      <c r="P2" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E3" s="4">
+        <v>20</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="G3" s="4">
+        <v>123456</v>
+      </c>
       <c r="H3" s="6" t="s">
-        <v>31</v>
+        <v>19</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="L3" s="7">
+        <v>500</v>
+      </c>
+      <c r="M3" s="6">
+        <v>50</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="O3">
+        <v>500</v>
+      </c>
+      <c r="P3" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Final Project - Add Product + Full Flow part 1
</commit_message>
<xml_diff>
--- a/src/test/java/haimai/datatest/dataTestProject.xlsx
+++ b/src/test/java/haimai/datatest/dataTestProject.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="64">
   <si>
     <t>name</t>
   </si>
@@ -204,15 +204,6 @@
     <t>Hai product 2</t>
   </si>
   <si>
-    <t>unit</t>
-  </si>
-  <si>
-    <t>kg</t>
-  </si>
-  <si>
-    <t>pc</t>
-  </si>
-  <si>
     <t>minPurchaseQty</t>
   </si>
   <si>
@@ -222,52 +213,13 @@
     <t>hai</t>
   </si>
   <si>
-    <t>barcode</t>
-  </si>
-  <si>
-    <t>galleryFilePath</t>
-  </si>
-  <si>
-    <t>galleryFileName</t>
-  </si>
-  <si>
-    <t>videoProvider</t>
-  </si>
-  <si>
-    <t>videoLink</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=JZ9pHBEUWPo</t>
-  </si>
-  <si>
-    <t>Vimeo</t>
-  </si>
-  <si>
-    <t>Dailymotion</t>
-  </si>
-  <si>
     <t>unitPrice</t>
   </si>
   <si>
     <t>discount</t>
   </si>
   <si>
-    <t>percent</t>
-  </si>
-  <si>
     <t>quantity</t>
-  </si>
-  <si>
-    <t>description</t>
-  </si>
-  <si>
-    <t>Description of Hai Product 1</t>
-  </si>
-  <si>
-    <t>Description of Hai Product 2</t>
-  </si>
-  <si>
-    <t>this is meta title</t>
   </si>
 </sst>
 </file>
@@ -981,28 +933,24 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q3"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="P7" sqref="P7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6:H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="13.5703125" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" customWidth="1"/>
-    <col min="4" max="4" width="6.28515625" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" customWidth="1"/>
-    <col min="6" max="7" width="7.7109375" customWidth="1"/>
-    <col min="8" max="8" width="18" customWidth="1"/>
-    <col min="9" max="9" width="14.85546875" customWidth="1"/>
-    <col min="10" max="10" width="15.85546875" customWidth="1"/>
-    <col min="11" max="11" width="14.28515625" customWidth="1"/>
-    <col min="12" max="12" width="8.7109375" customWidth="1"/>
-    <col min="13" max="13" width="13" customWidth="1"/>
+    <col min="1" max="2" width="15.85546875" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" customWidth="1"/>
+    <col min="5" max="5" width="7.7109375" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" customWidth="1"/>
+    <col min="7" max="7" width="13" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>54</v>
       </c>
@@ -1016,46 +964,19 @@
         <v>58</v>
       </c>
       <c r="E1" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="G1" s="4" t="s">
-        <v>64</v>
-      </c>
       <c r="H1" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="O1" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="P1" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="Q1" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>56</v>
       </c>
@@ -1065,50 +986,23 @@
       <c r="C2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="E2" s="4">
+      <c r="D2" s="4">
         <v>10</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="G2" s="4">
-        <v>98765</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="L2" s="7">
+      <c r="E2" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="F2" s="7">
         <v>200</v>
       </c>
-      <c r="M2" s="6">
+      <c r="G2" s="6">
         <v>30</v>
       </c>
-      <c r="N2" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="O2">
-        <v>1000</v>
-      </c>
-      <c r="P2" t="s">
-        <v>77</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="H2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>57</v>
       </c>
@@ -1118,50 +1012,24 @@
       <c r="C3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="4">
+        <v>20</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="E3" s="4">
-        <v>20</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="G3" s="4">
-        <v>123456</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="J3" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="K3" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="L3" s="7">
+      <c r="F3" s="7">
         <v>500</v>
       </c>
-      <c r="M3" s="6">
+      <c r="G3" s="6">
         <v>50</v>
       </c>
-      <c r="N3" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="O3">
+      <c r="H3">
         <v>500</v>
-      </c>
-      <c r="P3" t="s">
-        <v>78</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>79</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Final Project - Verify Data after adding and editing
</commit_message>
<xml_diff>
--- a/src/test/java/haimai/datatest/dataTestProject.xlsx
+++ b/src/test/java/haimai/datatest/dataTestProject.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="69">
   <si>
     <t>name</t>
   </si>
@@ -183,12 +183,6 @@
     <t>Wheel</t>
   </si>
   <si>
-    <t>Toy</t>
-  </si>
-  <si>
-    <t>Hot Categories</t>
-  </si>
-  <si>
     <t>catName</t>
   </si>
   <si>
@@ -220,6 +214,27 @@
   </si>
   <si>
     <t>quantity</t>
+  </si>
+  <si>
+    <t>unit</t>
+  </si>
+  <si>
+    <t>kg</t>
+  </si>
+  <si>
+    <t>pc</t>
+  </si>
+  <si>
+    <t>discountType</t>
+  </si>
+  <si>
+    <t>Flat</t>
+  </si>
+  <si>
+    <t>Percent</t>
+  </si>
+  <si>
+    <t>Demo category 1</t>
   </si>
 </sst>
 </file>
@@ -805,7 +820,7 @@
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A3"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -861,7 +876,7 @@
         <v>26</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>51</v>
+        <v>26</v>
       </c>
       <c r="C2" s="4">
         <v>123</v>
@@ -896,7 +911,7 @@
         <v>27</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>52</v>
+        <v>27</v>
       </c>
       <c r="C3" s="4">
         <v>456</v>
@@ -933,98 +948,116 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6:H7"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="15.85546875" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" customWidth="1"/>
-    <col min="4" max="4" width="21.42578125" customWidth="1"/>
-    <col min="5" max="5" width="7.7109375" customWidth="1"/>
-    <col min="6" max="6" width="11.5703125" customWidth="1"/>
-    <col min="7" max="7" width="13" customWidth="1"/>
-    <col min="8" max="8" width="13.42578125" customWidth="1"/>
+    <col min="3" max="4" width="16.5703125" customWidth="1"/>
+    <col min="5" max="5" width="21.42578125" customWidth="1"/>
+    <col min="6" max="6" width="7.7109375" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" customWidth="1"/>
+    <col min="8" max="9" width="13" customWidth="1"/>
+    <col min="10" max="10" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>56</v>
-      </c>
       <c r="B2" s="4" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E2" s="4">
         <v>10</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="F2" s="7">
+      <c r="F2" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="G2" s="7">
         <v>200</v>
       </c>
-      <c r="G2" s="6">
+      <c r="H2" s="6">
         <v>30</v>
       </c>
-      <c r="H2">
+      <c r="I2" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="J2">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>27</v>
+        <v>68</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E3" s="4">
         <v>20</v>
       </c>
-      <c r="E3" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="F3" s="7">
+      <c r="F3" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="G3" s="7">
         <v>500</v>
       </c>
-      <c r="G3" s="6">
+      <c r="H3" s="6">
         <v>50</v>
       </c>
-      <c r="H3">
+      <c r="I3" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="J3">
         <v>500</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Final Project Check detail on product on User page that has added from Admin page.
</commit_message>
<xml_diff>
--- a/src/test/java/haimai/datatest/dataTestProject.xlsx
+++ b/src/test/java/haimai/datatest/dataTestProject.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="68">
   <si>
     <t>name</t>
   </si>
@@ -172,9 +172,6 @@
   </si>
   <si>
     <t>Size</t>
-  </si>
-  <si>
-    <t>Digital</t>
   </si>
   <si>
     <t>Physical</t>
@@ -820,7 +817,7 @@
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -917,7 +914,7 @@
         <v>456</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>19</v>
@@ -938,7 +935,7 @@
         <v>31</v>
       </c>
       <c r="K3" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -951,7 +948,7 @@
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -967,54 +964,54 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>53</v>
-      </c>
       <c r="D1" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E1" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="F1" s="4" t="s">
-        <v>57</v>
-      </c>
       <c r="G1" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="J1" s="4" t="s">
         <v>60</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>68</v>
+        <v>26</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E2" s="4">
         <v>10</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G2" s="7">
         <v>200</v>
@@ -1023,7 +1020,7 @@
         <v>30</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J2">
         <v>15</v>
@@ -1031,22 +1028,22 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>4</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E3" s="4">
         <v>20</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G3" s="7">
         <v>500</v>
@@ -1055,7 +1052,7 @@
         <v>50</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J3">
         <v>500</v>

</xml_diff>